<commit_message>
Better text-graphics using Unicode
</commit_message>
<xml_diff>
--- a/notes/Array Content.xlsx
+++ b/notes/Array Content.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\repos\lasertank-python\notes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="11475" windowHeight="3930" tabRatio="851" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="11475" windowHeight="3930" tabRatio="851" activeTab="11"/>
   </bookViews>
   <sheets>
-    <sheet name="Minimal Attributes" sheetId="9" r:id="rId1"/>
-    <sheet name="Objects" sheetId="6" r:id="rId2"/>
+    <sheet name="Objects" sheetId="6" r:id="rId1"/>
+    <sheet name="Minimal Attributes" sheetId="9" r:id="rId2"/>
     <sheet name="C IDs" sheetId="1" r:id="rId3"/>
     <sheet name="BMP" sheetId="2" r:id="rId4"/>
     <sheet name="Language" sheetId="3" r:id="rId5"/>
@@ -20,7 +25,7 @@
     <sheet name="Tunnel IDs" sheetId="11" r:id="rId11"/>
     <sheet name="Custom IDs" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -3313,7 +3318,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3348,7 +3353,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3557,747 +3562,736 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="6" customWidth="1"/>
-    <col min="4" max="5" width="23" style="6" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.42578125" style="6" customWidth="1"/>
-    <col min="13" max="16384" width="8.7109375" style="6"/>
+    <col min="1" max="1" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="83.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="26.1" x14ac:dyDescent="0.6">
       <c r="A1" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>677</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+    </row>
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="33" t="s">
-        <v>661</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>682</v>
-      </c>
-      <c r="F2" s="33" t="s">
         <v>446</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="D2" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="E2" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="F2" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="G2" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="H2" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="I2" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="J2" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="K2" s="5" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="35" t="s">
-        <v>662</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>683</v>
-      </c>
-      <c r="F3" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="35" t="s">
+      <c r="C3" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="H3" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="35" t="s">
+      <c r="E3" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="H3" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="I3" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="M3" s="35" t="s">
+      <c r="J3" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="K3" s="8" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="38" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="H4" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="I4" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="M4" s="38" t="s">
+      <c r="J4" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="N4" s="40"/>
-    </row>
-    <row r="5" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+    </row>
+    <row r="5" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35" t="s">
-        <v>683</v>
-      </c>
-      <c r="F5" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="35" t="s">
+      <c r="C5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="35" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="H5" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="L5" s="35" t="s">
+      <c r="I5" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="M5" s="35" t="s">
+      <c r="J5" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="N5" s="37"/>
-    </row>
-    <row r="6" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+    </row>
+    <row r="6" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="38" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="H6" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="L6" s="38" t="s">
+      <c r="I6" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="J6" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="N6" s="40"/>
-    </row>
-    <row r="7" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
-        <v>663</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>662</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>683</v>
-      </c>
-      <c r="F7" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="35" t="s">
+    </row>
+    <row r="7" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="H7" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="35" t="s">
+      <c r="E7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="K7" s="35" t="s">
+      <c r="H7" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="L7" s="35" t="s">
+      <c r="I7" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="M7" s="35" t="s">
+      <c r="J7" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="N7" s="37" t="s">
+      <c r="K7" s="8" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+    <row r="8" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="E8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
+        <v>9</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="E9" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>10</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="E10" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>11</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>12</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>13</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>14</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>19</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>20</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>21</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>22</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>23</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="K20" s="8" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>662</v>
-      </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" s="31" t="s">
+      <c r="E21" s="7"/>
+      <c r="F21" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="K8" s="31" t="s">
+      <c r="H21" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="L8" s="31" t="s">
+      <c r="I21" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="M8" s="31" t="s">
+      <c r="J21" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="N8" s="32"/>
-    </row>
-    <row r="9" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="F9" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>440</v>
-      </c>
-      <c r="H9" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" s="35" t="s">
-        <v>433</v>
-      </c>
-      <c r="K9" s="35" t="s">
-        <v>435</v>
-      </c>
-      <c r="L9" s="35" t="s">
-        <v>436</v>
-      </c>
-      <c r="M9" s="35" t="s">
-        <v>434</v>
-      </c>
-      <c r="N9" s="37"/>
-    </row>
-    <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="F10" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="38" t="s">
-        <v>440</v>
-      </c>
-      <c r="H10" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" s="38" t="s">
-        <v>433</v>
-      </c>
-      <c r="K10" s="38" t="s">
-        <v>435</v>
-      </c>
-      <c r="L10" s="38" t="s">
-        <v>433</v>
-      </c>
-      <c r="M10" s="38" t="s">
-        <v>436</v>
-      </c>
-      <c r="N10" s="40"/>
-    </row>
-    <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
-        <v>664</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>662</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>683</v>
-      </c>
-      <c r="F11" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>440</v>
-      </c>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" s="35" t="s">
-        <v>441</v>
-      </c>
-      <c r="K11" s="35" t="s">
-        <v>435</v>
-      </c>
-      <c r="L11" s="35" t="s">
-        <v>433</v>
-      </c>
-      <c r="M11" s="35" t="s">
-        <v>442</v>
-      </c>
-      <c r="N11" s="37"/>
-    </row>
-    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="F12" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="38" t="s">
-        <v>440</v>
-      </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="38" t="s">
-        <v>443</v>
-      </c>
-      <c r="K12" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="L12" s="38" t="s">
-        <v>433</v>
-      </c>
-      <c r="M12" s="38" t="s">
-        <v>434</v>
-      </c>
-      <c r="N12" s="40"/>
-    </row>
-    <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="F13" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>440</v>
-      </c>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" s="35" t="s">
-        <v>433</v>
-      </c>
-      <c r="K13" s="35" t="s">
-        <v>444</v>
-      </c>
-      <c r="L13" s="35" t="s">
-        <v>443</v>
-      </c>
-      <c r="M13" s="35" t="s">
-        <v>434</v>
-      </c>
-      <c r="N13" s="37"/>
-    </row>
-    <row r="14" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="F14" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="38" t="s">
-        <v>440</v>
-      </c>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="38" t="s">
-        <v>433</v>
-      </c>
-      <c r="K14" s="38" t="s">
-        <v>435</v>
-      </c>
-      <c r="L14" s="38" t="s">
-        <v>441</v>
-      </c>
-      <c r="M14" s="38" t="s">
-        <v>444</v>
-      </c>
-      <c r="N14" s="40"/>
-    </row>
-    <row r="15" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" s="35" t="s">
-        <v>444</v>
-      </c>
-      <c r="K15" s="35" t="s">
-        <v>441</v>
-      </c>
-      <c r="L15" s="35" t="s">
-        <v>442</v>
-      </c>
-      <c r="M15" s="35" t="s">
-        <v>443</v>
-      </c>
-      <c r="N15" s="37"/>
-    </row>
-    <row r="16" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
-        <v>665</v>
-      </c>
-      <c r="B16" s="35" t="s">
-        <v>662</v>
-      </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" s="38" t="s">
-        <v>441</v>
-      </c>
-      <c r="K16" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="L16" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="M16" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="N16" s="40"/>
-    </row>
-    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" s="35" t="s">
-        <v>443</v>
-      </c>
-      <c r="K17" s="35" t="s">
-        <v>442</v>
-      </c>
-      <c r="L17" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="M17" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="N17" s="37"/>
-    </row>
-    <row r="18" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
-      <c r="B18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="K18" s="38" t="s">
-        <v>444</v>
-      </c>
-      <c r="L18" s="38" t="s">
-        <v>443</v>
-      </c>
-      <c r="M18" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="N18" s="40"/>
-    </row>
-    <row r="19" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="K19" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="L19" s="35" t="s">
-        <v>441</v>
-      </c>
-      <c r="M19" s="35" t="s">
-        <v>444</v>
-      </c>
-      <c r="N19" s="37"/>
-    </row>
-    <row r="20" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="40" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A22" s="9" t="s">
+    </row>
+    <row r="23" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A23" s="9" t="s">
         <v>464</v>
       </c>
-      <c r="B22" s="9"/>
-    </row>
-    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="41" t="s">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="41" t="s">
-        <v>667</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>670</v>
-      </c>
-      <c r="D23" s="41" t="s">
-        <v>680</v>
-      </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41" t="s">
+      <c r="C24" s="11" t="s">
         <v>447</v>
       </c>
-      <c r="G23" s="42" t="s">
+      <c r="D24" s="16" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>0</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="44"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="45" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>2</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45" t="s">
+      <c r="C26" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="G25" s="46"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
+      <c r="D26" s="13"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>3</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43" t="s">
+      <c r="C27" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="G26" s="44"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="45" t="s">
-        <v>668</v>
-      </c>
-      <c r="B27" s="35" t="s">
-        <v>662</v>
-      </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="45" t="s">
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>15</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="G27" s="46" t="s">
+      <c r="D28" s="13" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>16</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>17</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="D30" s="13"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>18</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>24</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45" t="s">
+      <c r="C32" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="G28" s="46"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="43" t="s">
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>25</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43" t="s">
-        <v>669</v>
-      </c>
-      <c r="G29" s="44"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
+      <c r="C33" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10" t="s">
         <v>448</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="46"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47" t="s">
-        <v>671</v>
-      </c>
-      <c r="D31" s="47" t="s">
-        <v>681</v>
-      </c>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47" t="s">
+      <c r="C34" s="10"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>710</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>711</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>450</v>
       </c>
-      <c r="G31" s="48"/>
-    </row>
-    <row r="33" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A33" s="9" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="41" t="s">
-        <v>672</v>
-      </c>
-      <c r="C34" s="41" t="s">
-        <v>674</v>
-      </c>
-      <c r="D34" s="42" t="s">
-        <v>675</v>
-      </c>
-      <c r="E34" s="49" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>461</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>673</v>
-      </c>
-      <c r="C35" s="35" t="s">
-        <v>662</v>
-      </c>
-      <c r="D35" s="35" t="s">
-        <v>662</v>
-      </c>
-      <c r="E35" s="50" t="s">
-        <v>679</v>
-      </c>
+      <c r="D35" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -4753,7 +4747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A33" sqref="A33:A36"/>
     </sheetView>
   </sheetViews>
@@ -5217,736 +5211,747 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="83.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7109375" style="6"/>
+    <col min="1" max="1" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" style="6" customWidth="1"/>
+    <col min="4" max="5" width="23" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.42578125" style="6" customWidth="1"/>
+    <col min="13" max="16384" width="8.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="B1" s="52" t="s">
+        <v>677</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>12</v>
       </c>
+      <c r="B2" s="33" t="s">
+        <v>661</v>
+      </c>
       <c r="C2" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="F2" s="33" t="s">
         <v>446</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="33" t="s">
         <v>454</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="H2" s="33" t="s">
         <v>428</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="I2" s="33" t="s">
         <v>429</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="J2" s="33" t="s">
         <v>430</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="K2" s="33" t="s">
         <v>438</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="L2" s="33" t="s">
         <v>431</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="M2" s="33" t="s">
         <v>432</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="N2" s="34" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="35" t="s">
+        <v>662</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>683</v>
+      </c>
+      <c r="F3" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="35" t="s">
         <v>439</v>
       </c>
-      <c r="E3" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="35" t="s">
         <v>439</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="K3" s="35" t="s">
         <v>439</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="L3" s="35" t="s">
         <v>439</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="M3" s="35" t="s">
         <v>439</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="N3" s="37" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
-        <v>4</v>
-      </c>
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8" t="s">
+      <c r="B4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="38" t="s">
         <v>445</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="K4" s="38" t="s">
         <v>445</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="L4" s="38" t="s">
         <v>445</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="M4" s="38" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A5" s="8">
-        <v>5</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="N4" s="40"/>
+    </row>
+    <row r="5" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35" t="s">
+        <v>683</v>
+      </c>
+      <c r="F5" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="35" t="s">
         <v>455</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="36"/>
+      <c r="I5" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="35" t="s">
         <v>433</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="K5" s="35" t="s">
         <v>435</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="L5" s="35" t="s">
         <v>433</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="M5" s="35" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A6" s="8">
-        <v>6</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="N5" s="37"/>
+    </row>
+    <row r="6" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="B6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="38" t="s">
         <v>440</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="K6" s="38" t="s">
         <v>440</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="L6" s="38" t="s">
         <v>440</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="M6" s="38" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A7" s="8">
+      <c r="N6" s="40"/>
+    </row>
+    <row r="7" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
+        <v>663</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>662</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>683</v>
+      </c>
+      <c r="F7" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>440</v>
+      </c>
+      <c r="H7" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="35" t="s">
+        <v>436</v>
+      </c>
+      <c r="K7" s="35" t="s">
+        <v>435</v>
+      </c>
+      <c r="L7" s="35" t="s">
+        <v>433</v>
+      </c>
+      <c r="M7" s="35" t="s">
+        <v>434</v>
+      </c>
+      <c r="N7" s="37" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>437</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>662</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>445</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>445</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>445</v>
+      </c>
+      <c r="M8" s="31" t="s">
+        <v>445</v>
+      </c>
+      <c r="N8" s="32"/>
+    </row>
+    <row r="9" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="F9" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>440</v>
+      </c>
+      <c r="H9" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="35" t="s">
+        <v>433</v>
+      </c>
+      <c r="K9" s="35" t="s">
+        <v>435</v>
+      </c>
+      <c r="L9" s="35" t="s">
+        <v>436</v>
+      </c>
+      <c r="M9" s="35" t="s">
+        <v>434</v>
+      </c>
+      <c r="N9" s="37"/>
+    </row>
+    <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="F10" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>440</v>
+      </c>
+      <c r="H10" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>433</v>
+      </c>
+      <c r="K10" s="38" t="s">
+        <v>435</v>
+      </c>
+      <c r="L10" s="38" t="s">
+        <v>433</v>
+      </c>
+      <c r="M10" s="38" t="s">
+        <v>436</v>
+      </c>
+      <c r="N10" s="40"/>
+    </row>
+    <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>664</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>662</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>683</v>
+      </c>
+      <c r="F11" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>440</v>
+      </c>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>441</v>
+      </c>
+      <c r="K11" s="35" t="s">
+        <v>435</v>
+      </c>
+      <c r="L11" s="35" t="s">
+        <v>433</v>
+      </c>
+      <c r="M11" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="N11" s="37"/>
+    </row>
+    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="F12" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>440</v>
+      </c>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>443</v>
+      </c>
+      <c r="K12" s="38" t="s">
+        <v>442</v>
+      </c>
+      <c r="L12" s="38" t="s">
+        <v>433</v>
+      </c>
+      <c r="M12" s="38" t="s">
+        <v>434</v>
+      </c>
+      <c r="N12" s="40"/>
+    </row>
+    <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="F13" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>440</v>
+      </c>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="35" t="s">
+        <v>433</v>
+      </c>
+      <c r="K13" s="35" t="s">
+        <v>444</v>
+      </c>
+      <c r="L13" s="35" t="s">
+        <v>443</v>
+      </c>
+      <c r="M13" s="35" t="s">
+        <v>434</v>
+      </c>
+      <c r="N13" s="37"/>
+    </row>
+    <row r="14" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="F14" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>440</v>
+      </c>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="38" t="s">
+        <v>433</v>
+      </c>
+      <c r="K14" s="38" t="s">
+        <v>435</v>
+      </c>
+      <c r="L14" s="38" t="s">
+        <v>441</v>
+      </c>
+      <c r="M14" s="38" t="s">
+        <v>444</v>
+      </c>
+      <c r="N14" s="40"/>
+    </row>
+    <row r="15" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" s="35" t="s">
+        <v>444</v>
+      </c>
+      <c r="K15" s="35" t="s">
+        <v>441</v>
+      </c>
+      <c r="L15" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="M15" s="35" t="s">
+        <v>443</v>
+      </c>
+      <c r="N15" s="37"/>
+    </row>
+    <row r="16" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
+        <v>665</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>662</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" s="38" t="s">
+        <v>441</v>
+      </c>
+      <c r="K16" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M16" s="38" t="s">
+        <v>442</v>
+      </c>
+      <c r="N16" s="40"/>
+    </row>
+    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="35" t="s">
+        <v>443</v>
+      </c>
+      <c r="K17" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="L17" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="M17" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="N17" s="37"/>
+    </row>
+    <row r="18" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="K18" s="38" t="s">
+        <v>444</v>
+      </c>
+      <c r="L18" s="38" t="s">
+        <v>443</v>
+      </c>
+      <c r="M18" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N18" s="40"/>
+    </row>
+    <row r="19" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="L19" s="35" t="s">
+        <v>441</v>
+      </c>
+      <c r="M19" s="35" t="s">
+        <v>444</v>
+      </c>
+      <c r="N19" s="37"/>
+    </row>
+    <row r="20" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="40" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A22" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>667</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>670</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>680</v>
+      </c>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41" t="s">
+        <v>447</v>
+      </c>
+      <c r="G23" s="42" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="44"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45" t="s">
+        <v>452</v>
+      </c>
+      <c r="G25" s="46"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43" t="s">
+        <v>453</v>
+      </c>
+      <c r="G26" s="44"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="45" t="s">
+        <v>668</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>662</v>
+      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="45" t="s">
+        <v>456</v>
+      </c>
+      <c r="G27" s="46" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45" t="s">
+        <v>451</v>
+      </c>
+      <c r="G28" s="46"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43" t="s">
+        <v>669</v>
+      </c>
+      <c r="G29" s="44"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="45" t="s">
+        <v>448</v>
+      </c>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="46"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="E7" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>434</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A8" s="8">
-        <v>8</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="E8" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A9" s="8">
-        <v>9</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="E9" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A10" s="8">
-        <v>10</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="E10" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>11</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="B31" s="47"/>
+      <c r="C31" s="47" t="s">
+        <v>671</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>681</v>
+      </c>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47" t="s">
+        <v>450</v>
+      </c>
+      <c r="G31" s="48"/>
+    </row>
+    <row r="33" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A33" s="9" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>443</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>442</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>13</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>443</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>14</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>19</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>442</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>20</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>21</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>443</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>442</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>22</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>443</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>23</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
+      <c r="B34" s="41" t="s">
+        <v>672</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>674</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>675</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="K20" s="8" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A23" s="9" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>425</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>447</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
-        <v>0</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="14"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
-        <v>2</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>452</v>
-      </c>
-      <c r="D26" s="13"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>3</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
-        <v>15</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>456</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
-        <v>16</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>457</v>
-      </c>
-      <c r="D29" s="13"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
-        <v>17</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>458</v>
-      </c>
-      <c r="D30" s="13"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
-        <v>18</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>459</v>
-      </c>
-      <c r="D31" s="13"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
-        <v>24</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="D32" s="13"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
-        <v>25</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="D33" s="13"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10" t="s">
-        <v>448</v>
-      </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>710</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>711</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>450</v>
-      </c>
-      <c r="D35" s="15"/>
+      <c r="B35" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>662</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>662</v>
+      </c>
+      <c r="E35" s="50" t="s">
+        <v>679</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -5954,8 +5959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:P75"/>
   <sheetViews>
-    <sheetView topLeftCell="D28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59:E75"/>
+    <sheetView topLeftCell="D34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q73" sqref="Q73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7312,9 +7317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15219,7 +15222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B383"/>
   <sheetViews>
-    <sheetView topLeftCell="A325" workbookViewId="0">
+    <sheetView topLeftCell="A202" workbookViewId="0">
       <selection activeCell="L79" sqref="L79"/>
     </sheetView>
   </sheetViews>
@@ -18529,7 +18532,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
GUI improvements including rendering a menubar and buttons panel. More standard levels added to the test coverage.
</commit_message>
<xml_diff>
--- a/notes/Array Content.xlsx
+++ b/notes/Array Content.xlsx
@@ -3643,7 +3643,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4203,9 +4203,6 @@
       <c r="K20" s="43"/>
       <c r="L20" s="43"/>
       <c r="M20" s="43"/>
-      <c r="N20" s="44" t="s">
-        <v>462</v>
-      </c>
     </row>
     <row r="22" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
@@ -4342,12 +4339,12 @@
       </c>
       <c r="G31" s="50"/>
     </row>
-    <row r="33" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="47" t="s">
         <v>12</v>
       </c>
@@ -4364,7 +4361,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="41" t="s">
         <v>461</v>
       </c>
@@ -4379,6 +4376,9 @@
       </c>
       <c r="E35" s="52" t="s">
         <v>678</v>
+      </c>
+      <c r="G35" s="44" t="s">
+        <v>462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>